<commit_message>
no more filings after 2019-05-10
</commit_message>
<xml_diff>
--- a/mfin_extraction/mfin_fillings.xlsx
+++ b/mfin_extraction/mfin_fillings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pysol\Desktop\projects\sec_filings\mfin_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9B5E8-4402-416A-B256-4ECD5EB9AD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241734D-A608-4442-800D-88908396B21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{552397D5-DD91-4AA9-9B31-1F531E5F5F72}"/>
   </bookViews>
@@ -423,7 +423,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -446,12 +446,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -460,6 +473,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -777,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF21D11D-DC14-4B7D-A608-ADA70796B033}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1467,7 +1486,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="A27" s="6">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1493,9 +1512,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
+      <c r="A28" s="7"/>
       <c r="B28">
         <v>1000209</v>
       </c>
@@ -1513,9 +1530,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
+      <c r="A29" s="7"/>
       <c r="B29">
         <v>1000209</v>
       </c>
@@ -1533,9 +1548,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
+      <c r="A30" s="7"/>
       <c r="B30">
         <v>1000209</v>
       </c>
@@ -1553,9 +1566,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
+      <c r="A31" s="7"/>
       <c r="B31">
         <v>1000209</v>
       </c>
@@ -1573,9 +1584,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
+      <c r="A32" s="7"/>
       <c r="B32">
         <v>1000209</v>
       </c>
@@ -1593,9 +1602,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
+      <c r="A33" s="7"/>
       <c r="B33">
         <v>1000209</v>
       </c>
@@ -1613,9 +1620,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
+      <c r="A34" s="7"/>
       <c r="B34">
         <v>1000209</v>
       </c>
@@ -1633,9 +1638,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
+      <c r="A35" s="7"/>
       <c r="B35">
         <v>1000209</v>
       </c>
@@ -1653,9 +1656,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
+      <c r="A36" s="7"/>
       <c r="B36">
         <v>1000209</v>
       </c>
@@ -1673,9 +1674,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
+      <c r="A37" s="7"/>
       <c r="B37">
         <v>1000209</v>
       </c>
@@ -1693,9 +1692,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
+      <c r="A38" s="7"/>
       <c r="B38">
         <v>1000209</v>
       </c>
@@ -1713,9 +1710,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
+      <c r="A39" s="7"/>
       <c r="B39">
         <v>1000209</v>
       </c>
@@ -1733,9 +1728,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
+      <c r="A40" s="7"/>
       <c r="B40">
         <v>1000209</v>
       </c>
@@ -1753,9 +1746,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
+      <c r="A41" s="7"/>
       <c r="B41">
         <v>1000209</v>
       </c>
@@ -1773,9 +1764,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
+      <c r="A42" s="7"/>
       <c r="B42">
         <v>1000209</v>
       </c>
@@ -1793,9 +1782,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
+      <c r="A43" s="7"/>
       <c r="B43">
         <v>1000209</v>
       </c>
@@ -1813,9 +1800,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
+      <c r="A44" s="7"/>
       <c r="B44">
         <v>1000209</v>
       </c>
@@ -1833,9 +1818,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
+      <c r="A45" s="7"/>
       <c r="B45">
         <v>1000209</v>
       </c>
@@ -1853,9 +1836,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
+      <c r="A46" s="7"/>
       <c r="B46">
         <v>1000209</v>
       </c>
@@ -1873,9 +1854,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
+      <c r="A47" s="7"/>
       <c r="B47">
         <v>1000209</v>
       </c>
@@ -1893,9 +1872,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
+      <c r="A48" s="7"/>
       <c r="B48">
         <v>1000209</v>
       </c>
@@ -1913,9 +1890,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
+      <c r="A49" s="7"/>
       <c r="B49">
         <v>1000209</v>
       </c>
@@ -1933,9 +1908,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
+      <c r="A50" s="7"/>
       <c r="B50">
         <v>1000209</v>
       </c>
@@ -1953,9 +1926,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
+      <c r="A51" s="7"/>
       <c r="B51">
         <v>1000209</v>
       </c>
@@ -1973,9 +1944,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
+      <c r="A52" s="7"/>
       <c r="B52">
         <v>1000209</v>
       </c>

</xml_diff>